<commit_message>
11-20 Video de EV
</commit_message>
<xml_diff>
--- a/Documentacao/QualidadedeSoftware/Planilha de Engenharia de Valor.xlsx
+++ b/Documentacao/QualidadedeSoftware/Planilha de Engenharia de Valor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" tabRatio="681"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" tabRatio="681" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="VisaoEstrategica" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,7 @@
     <sheet name="ValorxCusto(VC)" sheetId="3" r:id="rId3"/>
     <sheet name="VPI-ROI(VC)" sheetId="4" r:id="rId4"/>
     <sheet name="ValorxCustoAcc(VC)" sheetId="5" r:id="rId5"/>
-    <sheet name="Gráf1" sheetId="7" r:id="rId6"/>
-    <sheet name="Backlog" sheetId="6" r:id="rId7"/>
+    <sheet name="Backlog" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase">VisaoEstrategica!$B$6:$M$6</definedName>
@@ -632,6 +631,9 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -667,9 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,7 +878,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="4"/>
+            <c:idx val="11"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -908,7 +907,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="5"/>
+            <c:idx val="12"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -937,7 +936,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="6"/>
+            <c:idx val="13"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -970,7 +969,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="7"/>
+            <c:idx val="14"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -1003,7 +1002,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="8"/>
+            <c:idx val="15"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -1036,7 +1035,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="9"/>
+            <c:idx val="16"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -1069,7 +1068,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="10"/>
+            <c:idx val="17"/>
             <c:marker>
               <c:spPr>
                 <a:solidFill>
@@ -1267,7 +1266,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="4"/>
+              <c:idx val="11"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1308,7 +1307,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="5"/>
+              <c:idx val="12"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1349,7 +1348,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="6"/>
+              <c:idx val="13"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1390,7 +1389,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="7"/>
+              <c:idx val="14"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1431,7 +1430,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="8"/>
+              <c:idx val="15"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1472,7 +1471,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="9"/>
+              <c:idx val="16"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1513,7 +1512,7 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="10"/>
+              <c:idx val="17"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -2635,11 +2634,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-E3D6-463A-9178-2AD3C50494B0}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2661,11 +2656,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-E3D6-463A-9178-2AD3C50494B0}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2688,11 +2679,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-E3D6-463A-9178-2AD3C50494B0}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2715,11 +2702,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-E3D6-463A-9178-2AD3C50494B0}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2742,11 +2725,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-E3D6-463A-9178-2AD3C50494B0}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -2769,11 +2748,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000013-E3D6-463A-9178-2AD3C50494B0}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -2783,6 +2758,197 @@
               <a:solidFill>
                 <a:schemeClr val="accent5">
                   <a:lumMod val="60000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-E3D6-463A-9178-2AD3C50494B0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-E3D6-463A-9178-2AD3C50494B0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-E3D6-463A-9178-2AD3C50494B0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-E3D6-463A-9178-2AD3C50494B0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-E3D6-463A-9178-2AD3C50494B0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-E3D6-463A-9178-2AD3C50494B0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
                   <a:alpha val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -3747,257 +3913,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="422136863"/>
-        <c:axId val="422137279"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="422136863"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="422137279"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="422137279"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="422136863"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4607,520 +4523,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -5238,33 +4640,6 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9013209" cy="6198358"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5536,8 +4911,8 @@
   </sheetPr>
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5571,38 +4946,38 @@
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="22"/>
       <c r="AA2" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
       <c r="AA3" s="16">
         <v>2</v>
       </c>
@@ -5624,10 +4999,10 @@
       <c r="F4" s="19">
         <v>8</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="AA4" s="16">
         <v>3</v>
       </c>
@@ -5655,12 +5030,12 @@
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="31" t="s">
         <v>5</v>
       </c>
@@ -6439,8 +5814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6515,7 +5890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6559,18 +5934,18 @@
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="40"/>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>